<commit_message>
manually added dates for error 403 (2010)
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loowenwen/Desktop/Visual Code Studio/jtc-market-sentiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266DB0A3-0C24-744C-BC32-0A35242CDE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AEA55F-26F3-104A-A9B2-478BC3CABC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14940" yWindow="500" windowWidth="13860" windowHeight="15880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020 - 2024" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="2000 - 2004" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2010 - 2014'!$A$1:$C$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2010 - 2014'!$A$1:$C$79</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2015 - 2019'!$A$1:$C$503</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2020 - 2024'!$A$1:$C$590</definedName>
   </definedNames>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3528" uniqueCount="2330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3522" uniqueCount="2325">
   <si>
     <t>URLs</t>
   </si>
@@ -6557,12 +6557,6 @@
     <t>2010-05-21T20:30:40+0800</t>
   </si>
   <si>
-    <t>https://www.edgeprop.sg/hdb/139-jalan-bukit-merah</t>
-  </si>
-  <si>
-    <t>failed to retrieve the webpage: 403 Client Error: Forbidden for url: https://www.edgeprop.sg/hdb/139-jalan-bukit-merah</t>
-  </si>
-  <si>
     <t>https://www.businesstimes.com.sg/incoming/ura-acts-curb-use-soho-developers</t>
   </si>
   <si>
@@ -6578,9 +6572,6 @@
     <t>https://www.edgeprop.sg/property-news/sitting-goldmine-%E2%80%93-landed-housing-segment</t>
   </si>
   <si>
-    <t>failed to retrieve the webpage: 403 Client Error: Forbidden for url: https://www.edgeprop.sg/property-news/sitting-goldmine-%E2%80%93-landed-housing-segment</t>
-  </si>
-  <si>
     <t>https://www.businesstimes.com.sg/incoming/lawmakers-raise-flag-rising-business-costs</t>
   </si>
   <si>
@@ -6605,12 +6596,6 @@
     <t>2012-05-28T09:26:06+0800</t>
   </si>
   <si>
-    <t>https://www.edgeprop.sg/condo-apartment/crown-centre</t>
-  </si>
-  <si>
-    <t>failed to retrieve the webpage: 403 Client Error: Forbidden for url: https://www.edgeprop.sg/condo-apartment/crown-centre</t>
-  </si>
-  <si>
     <t>https://sbr.com.sg/residential-property/exclusive/possibly-one-last-luxury-condos-below-1000-psf-pasir-ris-launched</t>
   </si>
   <si>
@@ -6788,9 +6773,6 @@
     <t>https://www.edgeprop.sg/property-news/competition-heats-farrer-road-leedon-road</t>
   </si>
   <si>
-    <t>failed to retrieve the webpage: 403 Client Error: Forbidden for url: https://www.edgeprop.sg/property-news/competition-heats-farrer-road-leedon-road</t>
-  </si>
-  <si>
     <t>https://www.businesstimes.com.sg/companies-markets/geo-energy-ceo-tung-kum-hon-retire-dec-31</t>
   </si>
   <si>
@@ -6992,46 +6974,49 @@
     <t>https://www.edgeprop.sg/property-news/ho-bee%E2%80%99s-metropolis</t>
   </si>
   <si>
-    <t>failed to retrieve the webpage: 403 Client Error: Forbidden for url: https://www.edgeprop.sg/property-news/ho-bee%E2%80%99s-metropolis</t>
-  </si>
-  <si>
     <t>https://www.edgeprop.sg/property-news/new-lease-%E2%80%98awesomeness%E2%80%99</t>
   </si>
   <si>
-    <t>failed to retrieve the webpage: 403 Client Error: Forbidden for url: https://www.edgeprop.sg/property-news/new-lease-%E2%80%98awesomeness%E2%80%99</t>
-  </si>
-  <si>
     <t>https://www.edgeprop.sg/property-news/good-class-bungalow-35-mil</t>
   </si>
   <si>
-    <t>failed to retrieve the webpage: 403 Client Error: Forbidden for url: https://www.edgeprop.sg/property-news/good-class-bungalow-35-mil</t>
-  </si>
-  <si>
     <t>https://www.edgeprop.sg/property-news/prudential-tower-strata-unit-sale-2800-psf</t>
   </si>
   <si>
-    <t>failed to retrieve the webpage: 403 Client Error: Forbidden for url: https://www.edgeprop.sg/property-news/prudential-tower-strata-unit-sale-2800-psf</t>
-  </si>
-  <si>
     <t>https://www.edgeprop.sg/property-news/jewel-rangoon-road</t>
   </si>
   <si>
-    <t>failed to retrieve the webpage: 403 Client Error: Forbidden for url: https://www.edgeprop.sg/property-news/jewel-rangoon-road</t>
-  </si>
-  <si>
     <t>https://www.edgeprop.sg/property-news/shadow-d%E2%80%99leedon</t>
   </si>
   <si>
-    <t>failed to retrieve the webpage: 403 Client Error: Forbidden for url: https://www.edgeprop.sg/property-news/shadow-d%E2%80%99leedon</t>
-  </si>
-  <si>
     <t>https://www.edgeprop.sg/property-news/pricing-shock-iskandar%E2%80%99s-puteri-harbour</t>
   </si>
   <si>
-    <t>failed to retrieve the webpage: 403 Client Error: Forbidden for url: https://www.edgeprop.sg/property-news/pricing-shock-iskandar%E2%80%99s-puteri-harbour</t>
-  </si>
-  <si>
     <t>Quarter</t>
+  </si>
+  <si>
+    <t>2014-03-01T00:00:00+08:00</t>
+  </si>
+  <si>
+    <t>2014-10-06T00:00:00+08:00</t>
+  </si>
+  <si>
+    <t>2014-12-08T10:48:55+08:00</t>
+  </si>
+  <si>
+    <t>2014-10-13T00:00:00+08:00</t>
+  </si>
+  <si>
+    <t>2014-10-20T00:00:00+08:00</t>
+  </si>
+  <si>
+    <t>2014-10-27T10:50:58+08:00</t>
+  </si>
+  <si>
+    <t>2014-11-24T15:51:30+08:00</t>
+  </si>
+  <si>
+    <t>2014-10-20T13:31:07+08:00</t>
   </si>
 </sst>
 </file>
@@ -19458,10 +19443,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19523,815 +19508,815 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>2176</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2177</v>
+        <v>2176</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>2178</v>
+        <v>2177</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>2180</v>
+      </c>
+      <c r="B8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" t="s">
         <v>2181</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2182</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>2183</v>
+        <v>2182</v>
       </c>
       <c r="B9" t="s">
         <v>119</v>
       </c>
       <c r="C9" t="s">
-        <v>2184</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>2185</v>
+        <v>2184</v>
       </c>
       <c r="B10" t="s">
         <v>119</v>
       </c>
       <c r="C10" t="s">
-        <v>2186</v>
+        <v>2185</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>2187</v>
+        <v>2186</v>
       </c>
       <c r="B11" t="s">
         <v>119</v>
       </c>
       <c r="C11" t="s">
-        <v>2188</v>
+        <v>2187</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>2189</v>
+        <v>2188</v>
       </c>
       <c r="B12" t="s">
         <v>119</v>
       </c>
       <c r="C12" t="s">
-        <v>2190</v>
+        <v>2189</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
       <c r="B13" t="s">
         <v>119</v>
       </c>
       <c r="C13" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="B14" t="s">
         <v>119</v>
       </c>
       <c r="C14" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="B15" t="s">
         <v>119</v>
       </c>
       <c r="C15" t="s">
-        <v>2196</v>
+        <v>2195</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="B16" t="s">
         <v>119</v>
       </c>
       <c r="C16" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="B17" t="s">
         <v>119</v>
       </c>
       <c r="C17" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>2201</v>
+        <v>2200</v>
       </c>
       <c r="B18" t="s">
         <v>119</v>
       </c>
       <c r="C18" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>2203</v>
+        <v>2202</v>
       </c>
       <c r="B19" t="s">
         <v>119</v>
       </c>
       <c r="C19" t="s">
-        <v>2204</v>
+        <v>2203</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>2205</v>
+        <v>2204</v>
       </c>
       <c r="B20" t="s">
         <v>119</v>
       </c>
       <c r="C20" t="s">
-        <v>2206</v>
+        <v>2205</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>2207</v>
+        <v>2206</v>
       </c>
       <c r="B21" t="s">
         <v>119</v>
       </c>
       <c r="C21" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>2209</v>
+        <v>2208</v>
       </c>
       <c r="B22" t="s">
         <v>119</v>
       </c>
       <c r="C22" t="s">
-        <v>2210</v>
+        <v>2209</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>2210</v>
+      </c>
+      <c r="B23" t="s">
+        <v>301</v>
+      </c>
+      <c r="C23" t="s">
         <v>2211</v>
-      </c>
-      <c r="B23" t="s">
-        <v>119</v>
-      </c>
-      <c r="C23" t="s">
-        <v>2212</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>2212</v>
+      </c>
+      <c r="B24" t="s">
+        <v>301</v>
+      </c>
+      <c r="C24" t="s">
         <v>2213</v>
-      </c>
-      <c r="B24" t="s">
-        <v>119</v>
-      </c>
-      <c r="C24" t="s">
-        <v>2214</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>2214</v>
+      </c>
+      <c r="B25" t="s">
+        <v>301</v>
+      </c>
+      <c r="C25" t="s">
         <v>2215</v>
-      </c>
-      <c r="B25" t="s">
-        <v>301</v>
-      </c>
-      <c r="C25" t="s">
-        <v>2216</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>2216</v>
+      </c>
+      <c r="B26" t="s">
+        <v>301</v>
+      </c>
+      <c r="C26" t="s">
         <v>2217</v>
-      </c>
-      <c r="B26" t="s">
-        <v>301</v>
-      </c>
-      <c r="C26" t="s">
-        <v>2218</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>2218</v>
+      </c>
+      <c r="B27" t="s">
+        <v>301</v>
+      </c>
+      <c r="C27" t="s">
         <v>2219</v>
-      </c>
-      <c r="B27" t="s">
-        <v>301</v>
-      </c>
-      <c r="C27" t="s">
-        <v>2220</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>2220</v>
+      </c>
+      <c r="B28" t="s">
+        <v>301</v>
+      </c>
+      <c r="C28" t="s">
         <v>2221</v>
-      </c>
-      <c r="B28" t="s">
-        <v>301</v>
-      </c>
-      <c r="C28" t="s">
-        <v>2222</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>2222</v>
+      </c>
+      <c r="B29" t="s">
+        <v>301</v>
+      </c>
+      <c r="C29" t="s">
         <v>2223</v>
-      </c>
-      <c r="B29" t="s">
-        <v>301</v>
-      </c>
-      <c r="C29" t="s">
-        <v>2224</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>2224</v>
+      </c>
+      <c r="B30" t="s">
+        <v>301</v>
+      </c>
+      <c r="C30" t="s">
         <v>2225</v>
-      </c>
-      <c r="B30" t="s">
-        <v>301</v>
-      </c>
-      <c r="C30" t="s">
-        <v>2226</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>2226</v>
+      </c>
+      <c r="B31" t="s">
+        <v>301</v>
+      </c>
+      <c r="C31" t="s">
         <v>2227</v>
-      </c>
-      <c r="B31" t="s">
-        <v>301</v>
-      </c>
-      <c r="C31" t="s">
-        <v>2228</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>2228</v>
+      </c>
+      <c r="B32" t="s">
+        <v>301</v>
+      </c>
+      <c r="C32" t="s">
         <v>2229</v>
-      </c>
-      <c r="B32" t="s">
-        <v>301</v>
-      </c>
-      <c r="C32" t="s">
-        <v>2230</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>2230</v>
+      </c>
+      <c r="B33" t="s">
+        <v>301</v>
+      </c>
+      <c r="C33" t="s">
         <v>2231</v>
-      </c>
-      <c r="B33" t="s">
-        <v>301</v>
-      </c>
-      <c r="C33" t="s">
-        <v>2232</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>2232</v>
+      </c>
+      <c r="B34" t="s">
+        <v>301</v>
+      </c>
+      <c r="C34" t="s">
         <v>2233</v>
-      </c>
-      <c r="B34" t="s">
-        <v>301</v>
-      </c>
-      <c r="C34" t="s">
-        <v>2234</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>2234</v>
+      </c>
+      <c r="B35" t="s">
+        <v>301</v>
+      </c>
+      <c r="C35" t="s">
         <v>2235</v>
-      </c>
-      <c r="B35" t="s">
-        <v>301</v>
-      </c>
-      <c r="C35" t="s">
-        <v>2236</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>2236</v>
+      </c>
+      <c r="B36" t="s">
+        <v>301</v>
+      </c>
+      <c r="C36" t="s">
         <v>2237</v>
-      </c>
-      <c r="B36" t="s">
-        <v>301</v>
-      </c>
-      <c r="C36" t="s">
-        <v>2238</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>2238</v>
+      </c>
+      <c r="B37" t="s">
+        <v>301</v>
+      </c>
+      <c r="C37" t="s">
         <v>2239</v>
-      </c>
-      <c r="B37" t="s">
-        <v>301</v>
-      </c>
-      <c r="C37" t="s">
-        <v>2240</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>2240</v>
+      </c>
+      <c r="B38" t="s">
+        <v>301</v>
+      </c>
+      <c r="C38" t="s">
         <v>2241</v>
-      </c>
-      <c r="B38" t="s">
-        <v>301</v>
-      </c>
-      <c r="C38" t="s">
-        <v>2242</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="B39" t="s">
         <v>301</v>
       </c>
       <c r="C39" t="s">
-        <v>2244</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>2245</v>
+        <v>2243</v>
       </c>
       <c r="B40" t="s">
-        <v>301</v>
+        <v>603</v>
       </c>
       <c r="C40" t="s">
-        <v>2246</v>
+        <v>2244</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>2247</v>
+        <v>2245</v>
       </c>
       <c r="B41" t="s">
-        <v>301</v>
+        <v>603</v>
       </c>
       <c r="C41" t="s">
-        <v>2248</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>2249</v>
+        <v>2247</v>
       </c>
       <c r="B42" t="s">
         <v>603</v>
       </c>
       <c r="C42" t="s">
-        <v>2250</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>2251</v>
+        <v>2249</v>
       </c>
       <c r="B43" t="s">
         <v>603</v>
       </c>
       <c r="C43" t="s">
-        <v>2252</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>2253</v>
+        <v>2251</v>
       </c>
       <c r="B44" t="s">
         <v>603</v>
       </c>
       <c r="C44" t="s">
-        <v>2254</v>
+        <v>2252</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>2255</v>
+        <v>2253</v>
       </c>
       <c r="B45" t="s">
-        <v>603</v>
+        <v>301</v>
       </c>
       <c r="C45" t="s">
-        <v>2256</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>2257</v>
+        <v>2255</v>
       </c>
       <c r="B46" t="s">
-        <v>603</v>
+        <v>301</v>
       </c>
       <c r="C46" t="s">
-        <v>2258</v>
+        <v>2256</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>2259</v>
+        <v>2257</v>
       </c>
       <c r="B47" t="s">
         <v>301</v>
       </c>
       <c r="C47" t="s">
-        <v>2260</v>
+        <v>2258</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>2261</v>
+        <v>2259</v>
       </c>
       <c r="B48" t="s">
         <v>301</v>
       </c>
       <c r="C48" t="s">
-        <v>2262</v>
+        <v>2260</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>2263</v>
+        <v>2261</v>
       </c>
       <c r="B49" t="s">
         <v>301</v>
       </c>
       <c r="C49" t="s">
-        <v>2264</v>
+        <v>2262</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>2265</v>
+        <v>2263</v>
       </c>
       <c r="B50" t="s">
         <v>301</v>
       </c>
       <c r="C50" t="s">
-        <v>2266</v>
+        <v>2264</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>2267</v>
+        <v>2265</v>
       </c>
       <c r="B51" t="s">
         <v>301</v>
       </c>
       <c r="C51" t="s">
-        <v>2268</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>2269</v>
+        <v>2267</v>
       </c>
       <c r="B52" t="s">
         <v>301</v>
       </c>
       <c r="C52" t="s">
-        <v>2270</v>
+        <v>2268</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>2271</v>
+        <v>2269</v>
       </c>
       <c r="B53" t="s">
         <v>301</v>
       </c>
       <c r="C53" t="s">
-        <v>2272</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>2273</v>
+        <v>2271</v>
       </c>
       <c r="B54" t="s">
         <v>301</v>
       </c>
       <c r="C54" t="s">
-        <v>2274</v>
+        <v>2272</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>2275</v>
+        <v>2273</v>
       </c>
       <c r="B55" t="s">
         <v>301</v>
       </c>
       <c r="C55" t="s">
-        <v>2276</v>
+        <v>2274</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>2277</v>
+        <v>2275</v>
       </c>
       <c r="B56" t="s">
         <v>301</v>
       </c>
       <c r="C56" t="s">
-        <v>2278</v>
+        <v>2276</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>2279</v>
+        <v>2277</v>
       </c>
       <c r="B57" t="s">
         <v>301</v>
       </c>
       <c r="C57" t="s">
-        <v>2280</v>
+        <v>2278</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>2281</v>
+        <v>2279</v>
       </c>
       <c r="B58" t="s">
         <v>301</v>
       </c>
       <c r="C58" t="s">
-        <v>2282</v>
+        <v>2280</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>2283</v>
+        <v>2281</v>
       </c>
       <c r="B59" t="s">
         <v>301</v>
       </c>
       <c r="C59" t="s">
-        <v>2284</v>
+        <v>2282</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>2285</v>
+        <v>2283</v>
       </c>
       <c r="B60" t="s">
         <v>301</v>
       </c>
       <c r="C60" t="s">
-        <v>2286</v>
+        <v>2284</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>2287</v>
+        <v>2285</v>
       </c>
       <c r="B61" t="s">
         <v>301</v>
       </c>
       <c r="C61" t="s">
-        <v>2288</v>
+        <v>2286</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>2289</v>
+        <v>2287</v>
       </c>
       <c r="B62" t="s">
         <v>301</v>
       </c>
       <c r="C62" t="s">
-        <v>2290</v>
+        <v>2288</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>2291</v>
+        <v>2289</v>
       </c>
       <c r="B63" t="s">
         <v>301</v>
       </c>
       <c r="C63" t="s">
-        <v>2292</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>2293</v>
+        <v>2291</v>
       </c>
       <c r="B64" t="s">
         <v>301</v>
       </c>
       <c r="C64" t="s">
-        <v>2294</v>
+        <v>2292</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>2295</v>
+        <v>2293</v>
       </c>
       <c r="B65" t="s">
         <v>301</v>
       </c>
       <c r="C65" t="s">
-        <v>2296</v>
+        <v>2294</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>2297</v>
+        <v>2295</v>
       </c>
       <c r="B66" t="s">
-        <v>301</v>
+        <v>603</v>
       </c>
       <c r="C66" t="s">
-        <v>2298</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>2299</v>
+        <v>2297</v>
       </c>
       <c r="B67" t="s">
-        <v>301</v>
+        <v>603</v>
       </c>
       <c r="C67" t="s">
-        <v>2300</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>2301</v>
+        <v>2299</v>
       </c>
       <c r="B68" t="s">
         <v>603</v>
       </c>
       <c r="C68" t="s">
-        <v>2302</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>2303</v>
+        <v>2301</v>
       </c>
       <c r="B69" t="s">
         <v>603</v>
       </c>
       <c r="C69" t="s">
-        <v>2304</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>2305</v>
+        <v>2303</v>
       </c>
       <c r="B70" t="s">
         <v>603</v>
       </c>
       <c r="C70" t="s">
-        <v>2306</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>2307</v>
+        <v>2305</v>
       </c>
       <c r="B71" t="s">
         <v>603</v>
       </c>
       <c r="C71" t="s">
-        <v>2308</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>2309</v>
+        <v>2307</v>
       </c>
       <c r="B72" t="s">
         <v>603</v>
       </c>
       <c r="C72" t="s">
-        <v>2310</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>2311</v>
+        <v>2309</v>
       </c>
       <c r="B73" t="s">
-        <v>603</v>
+        <v>787</v>
       </c>
       <c r="C73" t="s">
-        <v>2312</v>
+        <v>2319</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>2313</v>
+        <v>2310</v>
       </c>
       <c r="B74" t="s">
-        <v>603</v>
+        <v>787</v>
       </c>
       <c r="C74" t="s">
-        <v>2314</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>2315</v>
+        <v>2311</v>
       </c>
       <c r="B75" t="s">
         <v>787</v>
       </c>
       <c r="C75" t="s">
-        <v>2316</v>
+        <v>2320</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>2317</v>
+        <v>2312</v>
       </c>
       <c r="B76" t="s">
         <v>787</v>
       </c>
       <c r="C76" t="s">
-        <v>2318</v>
+        <v>2321</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>2319</v>
+        <v>2313</v>
       </c>
       <c r="B77" t="s">
         <v>787</v>
       </c>
       <c r="C77" t="s">
-        <v>2320</v>
+        <v>2322</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>2321</v>
+        <v>2314</v>
       </c>
       <c r="B78" t="s">
         <v>787</v>
       </c>
       <c r="C78" t="s">
-        <v>2322</v>
+        <v>2323</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>2323</v>
+        <v>2315</v>
       </c>
       <c r="B79" t="s">
         <v>787</v>
@@ -20340,30 +20325,8 @@
         <v>2324</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>2325</v>
-      </c>
-      <c r="B80" t="s">
-        <v>787</v>
-      </c>
-      <c r="C80" t="s">
-        <v>2326</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>2327</v>
-      </c>
-      <c r="B81" t="s">
-        <v>787</v>
-      </c>
-      <c r="C81" t="s">
-        <v>2328</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C81" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
+  <autoFilter ref="A1:C79" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -20384,7 +20347,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2329</v>
+        <v>2316</v>
       </c>
     </row>
   </sheetData>
@@ -20408,7 +20371,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2329</v>
+        <v>2316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>